<commit_message>
Updated output files (which we're archiving in Github) Moved coupon_oringin in Positions.xml Fixes to grind programs duplicated from AutoGrind
</commit_message>
<xml_diff>
--- a/Data/10_inspect_all_1000mm_2022-06-21T17-21-30.xlsx
+++ b/Data/10_inspect_all_1000mm_2022-06-21T17-21-30.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nedlecky\GitHub\LEonard\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{68802CA4-7BBB-4623-BCFB-C1DF5F59733F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F79C831-62B5-455C-9015-6EBAECFD36C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37230" yWindow="405" windowWidth="36225" windowHeight="19620"/>
+    <workbookView xWindow="915" yWindow="45" windowWidth="36225" windowHeight="19620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="10_inspect_all_2022-06-21T17-21" sheetId="1" r:id="rId1"/>
@@ -744,7 +744,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -5994,7 +5994,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="2.6890110073820389E-2"/>
+          <c:y val="5.2967479674796751E-2"/>
+          <c:w val="0.95976442435141462"/>
+          <c:h val="0.90384130337366364"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -11426,10 +11436,10 @@
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11458,16 +11468,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>428624</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11507,10 +11517,10 @@
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>261937</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11539,16 +11549,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>133351</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>190501</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11874,10 +11884,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X214"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U1" sqref="U1:V1048576"/>
     </sheetView>
   </sheetViews>
@@ -27734,7 +27744,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -27749,10 +27759,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="V41" sqref="V41"/>
     </sheetView>
   </sheetViews>

</xml_diff>